<commit_message>
project 1 Bayeisan regression
</commit_message>
<xml_diff>
--- a/Project1/DataProcessed/cleaned data.xlsx
+++ b/Project1/DataProcessed/cleaned data.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t xml:space="preserve">newid</t>
   </si>
@@ -74,16 +74,13 @@
     <t xml:space="preserve">Healthy</t>
   </si>
   <si>
-    <t xml:space="preserve">Some college</t>
+    <t xml:space="preserve">some college</t>
   </si>
   <si>
     <t xml:space="preserve">Obsese</t>
   </si>
   <si>
     <t xml:space="preserve">Overweight</t>
-  </si>
-  <si>
-    <t xml:space="preserve">some college</t>
   </si>
   <si>
     <t xml:space="preserve">Graduate, Post Graduate</t>
@@ -695,7 +692,7 @@
         <v>5.91506853955031</v>
       </c>
       <c r="Q5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R5" t="s">
         <v>21</v>
@@ -751,7 +748,7 @@
         <v>5.73074954293774</v>
       </c>
       <c r="Q6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R6" t="s">
         <v>21</v>
@@ -863,7 +860,7 @@
         <v>6.6328036172327</v>
       </c>
       <c r="Q8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R8" t="s">
         <v>19</v>
@@ -919,7 +916,7 @@
         <v>6.3060863324184</v>
       </c>
       <c r="Q9" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R9" t="s">
         <v>22</v>
@@ -975,7 +972,7 @@
         <v>7.45467688072823</v>
       </c>
       <c r="Q10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R10" t="s">
         <v>19</v>
@@ -1087,7 +1084,7 @@
         <v>6.54735397893718</v>
       </c>
       <c r="Q12" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R12" t="s">
         <v>19</v>
@@ -1255,7 +1252,7 @@
         <v>5.91177210877048</v>
       </c>
       <c r="Q15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R15" t="s">
         <v>19</v>
@@ -1367,7 +1364,7 @@
         <v>6.15423518327498</v>
       </c>
       <c r="Q17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R17" t="s">
         <v>19</v>
@@ -1423,7 +1420,7 @@
         <v>5.42224705940926</v>
       </c>
       <c r="Q18" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R18" t="s">
         <v>19</v>
@@ -1479,7 +1476,7 @@
         <v>5.3606499938335</v>
       </c>
       <c r="Q19" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R19" t="s">
         <v>19</v>
@@ -1591,7 +1588,7 @@
         <v>4.85356409949217</v>
       </c>
       <c r="Q21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R21" t="s">
         <v>22</v>
@@ -1647,7 +1644,7 @@
         <v>6.47510407657533</v>
       </c>
       <c r="Q22" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R22" t="s">
         <v>22</v>
@@ -1815,7 +1812,7 @@
         <v>5.14006361001915</v>
       </c>
       <c r="Q25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R25" t="s">
         <v>19</v>
@@ -1927,7 +1924,7 @@
         <v>6.44829990223443</v>
       </c>
       <c r="Q27" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R27" t="s">
         <v>21</v>
@@ -2039,7 +2036,7 @@
         <v>5.90434472551118</v>
       </c>
       <c r="Q29" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R29" t="s">
         <v>19</v>
@@ -2151,7 +2148,7 @@
         <v>5.66389532358916</v>
       </c>
       <c r="Q31" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R31" t="s">
         <v>22</v>
@@ -2266,7 +2263,7 @@
         <v>20</v>
       </c>
       <c r="R33" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="34">
@@ -2319,7 +2316,7 @@
         <v>6.5674596744159</v>
       </c>
       <c r="Q34" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R34" t="s">
         <v>19</v>
@@ -2375,7 +2372,7 @@
         <v>5.38860089981537</v>
       </c>
       <c r="Q35" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R35" t="s">
         <v>19</v>
@@ -2599,7 +2596,7 @@
         <v>5.93704955555319</v>
       </c>
       <c r="Q39" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R39" t="s">
         <v>19</v>
@@ -2711,7 +2708,7 @@
         <v>6.74062023560554</v>
       </c>
       <c r="Q41" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R41" t="s">
         <v>19</v>
@@ -2823,7 +2820,7 @@
         <v>7.04157553838064</v>
       </c>
       <c r="Q43" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R43" t="s">
         <v>22</v>
@@ -3103,7 +3100,7 @@
         <v>6.16137407403586</v>
       </c>
       <c r="Q48" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R48" t="s">
         <v>21</v>
@@ -3271,7 +3268,7 @@
         <v>6.07741715058637</v>
       </c>
       <c r="Q51" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R51" t="s">
         <v>22</v>
@@ -3327,7 +3324,7 @@
         <v>6.95110570791636</v>
       </c>
       <c r="Q52" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R52" t="s">
         <v>19</v>
@@ -3439,7 +3436,7 @@
         <v>6.71559533781077</v>
       </c>
       <c r="Q54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R54" t="s">
         <v>22</v>
@@ -3495,7 +3492,7 @@
         <v>4.82831855089072</v>
       </c>
       <c r="Q55" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R55" t="s">
         <v>22</v>
@@ -3663,7 +3660,7 @@
         <v>6.54719410858083</v>
       </c>
       <c r="Q58" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R58" t="s">
         <v>22</v>
@@ -3775,7 +3772,7 @@
         <v>6.65786734825534</v>
       </c>
       <c r="Q60" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R60" t="s">
         <v>19</v>
@@ -3887,7 +3884,7 @@
         <v>6.23783920939283</v>
       </c>
       <c r="Q62" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R62" t="s">
         <v>22</v>
@@ -4167,7 +4164,7 @@
         <v>6.0447340608995</v>
       </c>
       <c r="Q67" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R67" t="s">
         <v>19</v>
@@ -4335,7 +4332,7 @@
         <v>6.06862218674143</v>
       </c>
       <c r="Q70" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R70" t="s">
         <v>22</v>
@@ -4503,7 +4500,7 @@
         <v>7.23173983738383</v>
       </c>
       <c r="Q73" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R73" t="s">
         <v>21</v>
@@ -4615,7 +4612,7 @@
         <v>6.21423618226995</v>
       </c>
       <c r="Q75" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R75" t="s">
         <v>22</v>
@@ -4674,7 +4671,7 @@
         <v>18</v>
       </c>
       <c r="R76" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="77">
@@ -4839,7 +4836,7 @@
         <v>6.63070108733266</v>
       </c>
       <c r="Q79" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R79" t="s">
         <v>19</v>
@@ -5119,7 +5116,7 @@
         <v>5.47473987185067</v>
       </c>
       <c r="Q84" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R84" t="s">
         <v>21</v>
@@ -5287,7 +5284,7 @@
         <v>6.41784503408962</v>
       </c>
       <c r="Q87" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R87" t="s">
         <v>19</v>
@@ -5455,7 +5452,7 @@
         <v>5.9268439650035</v>
       </c>
       <c r="Q90" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R90" t="s">
         <v>21</v>
@@ -5511,7 +5508,7 @@
         <v>6.35741399630397</v>
       </c>
       <c r="Q91" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R91" t="s">
         <v>21</v>
@@ -5567,7 +5564,7 @@
         <v>5.51277154759601</v>
       </c>
       <c r="Q92" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R92" t="s">
         <v>22</v>
@@ -5679,7 +5676,7 @@
         <v>6.21190410392192</v>
       </c>
       <c r="Q94" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R94" t="s">
         <v>19</v>
@@ -5735,7 +5732,7 @@
         <v>5.89371475820086</v>
       </c>
       <c r="Q95" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R95" t="s">
         <v>19</v>
@@ -5959,7 +5956,7 @@
         <v>6.15881897354866</v>
       </c>
       <c r="Q99" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R99" t="s">
         <v>22</v>
@@ -6015,7 +6012,7 @@
         <v>6.47553606067054</v>
       </c>
       <c r="Q100" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R100" t="s">
         <v>22</v>
@@ -6071,7 +6068,7 @@
         <v>6.25507018786438</v>
       </c>
       <c r="Q101" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R101" t="s">
         <v>21</v>
@@ -6127,7 +6124,7 @@
         <v>6.19408250939215</v>
       </c>
       <c r="Q102" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R102" t="s">
         <v>19</v>
@@ -6183,7 +6180,7 @@
         <v>6.19953726172662</v>
       </c>
       <c r="Q103" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R103" t="s">
         <v>22</v>
@@ -6239,7 +6236,7 @@
         <v>5.49512780652934</v>
       </c>
       <c r="Q104" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R104" t="s">
         <v>19</v>
@@ -6295,7 +6292,7 @@
         <v>5.4571799516079</v>
       </c>
       <c r="Q105" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R105" t="s">
         <v>22</v>
@@ -6407,10 +6404,10 @@
         <v>6.02189130024105</v>
       </c>
       <c r="Q107" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R107" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="108">
@@ -6463,7 +6460,7 @@
         <v>5.75301319732104</v>
       </c>
       <c r="Q108" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R108" t="s">
         <v>19</v>
@@ -6575,7 +6572,7 @@
         <v>6.68495961002484</v>
       </c>
       <c r="Q110" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R110" t="s">
         <v>19</v>
@@ -6743,7 +6740,7 @@
         <v>6.51496598753096</v>
       </c>
       <c r="Q113" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R113" t="s">
         <v>19</v>
@@ -6855,7 +6852,7 @@
         <v>7.00249085464221</v>
       </c>
       <c r="Q115" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R115" t="s">
         <v>19</v>
@@ -7471,7 +7468,7 @@
         <v>4.94285264856179</v>
       </c>
       <c r="Q126" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R126" t="s">
         <v>22</v>
@@ -7527,7 +7524,7 @@
         <v>6.36791271009185</v>
       </c>
       <c r="Q127" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R127" t="s">
         <v>19</v>
@@ -7583,7 +7580,7 @@
         <v>6.28843768407284</v>
       </c>
       <c r="Q128" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R128" t="s">
         <v>21</v>
@@ -7695,7 +7692,7 @@
         <v>6.39153531472112</v>
       </c>
       <c r="Q130" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R130" t="s">
         <v>22</v>
@@ -7751,7 +7748,7 @@
         <v>6.6928562080981</v>
       </c>
       <c r="Q131" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R131" t="s">
         <v>21</v>
@@ -7807,7 +7804,7 @@
         <v>5.85662607376838</v>
       </c>
       <c r="Q132" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R132" t="s">
         <v>22</v>
@@ -8031,7 +8028,7 @@
         <v>6.8387820609092</v>
       </c>
       <c r="Q136" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R136" t="s">
         <v>19</v>
@@ -8087,7 +8084,7 @@
         <v>6.01097067211837</v>
       </c>
       <c r="Q137" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R137" t="s">
         <v>22</v>
@@ -8255,7 +8252,7 @@
         <v>6.64921245190291</v>
       </c>
       <c r="Q140" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R140" t="s">
         <v>22</v>
@@ -8311,7 +8308,7 @@
         <v>6.24704624767335</v>
       </c>
       <c r="Q141" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R141" t="s">
         <v>19</v>
@@ -8535,7 +8532,7 @@
         <v>6.18284178880415</v>
       </c>
       <c r="Q145" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R145" t="s">
         <v>22</v>
@@ -8591,7 +8588,7 @@
         <v>5.29767054340304</v>
       </c>
       <c r="Q146" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R146" t="s">
         <v>19</v>
@@ -8703,7 +8700,7 @@
         <v>5.18960012337885</v>
       </c>
       <c r="Q148" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R148" t="s">
         <v>19</v>
@@ -8871,7 +8868,7 @@
         <v>6.38660244383076</v>
       </c>
       <c r="Q151" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R151" t="s">
         <v>19</v>
@@ -8927,7 +8924,7 @@
         <v>6.38620180758013</v>
       </c>
       <c r="Q152" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R152" t="s">
         <v>19</v>
@@ -9039,7 +9036,7 @@
         <v>5.44943120555278</v>
       </c>
       <c r="Q154" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R154" t="s">
         <v>22</v>
@@ -9095,7 +9092,7 @@
         <v>5.10537528834539</v>
       </c>
       <c r="Q155" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R155" t="s">
         <v>22</v>
@@ -9207,7 +9204,7 @@
         <v>6.48417170333526</v>
       </c>
       <c r="Q157" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R157" t="s">
         <v>19</v>
@@ -9322,7 +9319,7 @@
         <v>20</v>
       </c>
       <c r="R159" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="160">
@@ -9543,7 +9540,7 @@
         <v>5.57587834003661</v>
       </c>
       <c r="Q163" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R163" t="s">
         <v>22</v>
@@ -9599,7 +9596,7 @@
         <v>6.31392445857727</v>
       </c>
       <c r="Q164" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R164" t="s">
         <v>21</v>
@@ -9655,7 +9652,7 @@
         <v>5.77304191843182</v>
       </c>
       <c r="Q165" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R165" t="s">
         <v>19</v>
@@ -9711,7 +9708,7 @@
         <v>6.40709159750642</v>
       </c>
       <c r="Q166" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R166" t="s">
         <v>19</v>
@@ -9879,7 +9876,7 @@
         <v>6.38052203386988</v>
       </c>
       <c r="Q169" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R169" t="s">
         <v>19</v>
@@ -9935,7 +9932,7 @@
         <v>6.85936143711664</v>
       </c>
       <c r="Q170" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R170" t="s">
         <v>19</v>
@@ -9991,7 +9988,7 @@
         <v>7.35253858138958</v>
       </c>
       <c r="Q171" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R171" t="s">
         <v>22</v>
@@ -10159,7 +10156,7 @@
         <v>6.58313002163683</v>
       </c>
       <c r="Q174" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R174" t="s">
         <v>22</v>
@@ -10215,7 +10212,7 @@
         <v>5.27361402205008</v>
       </c>
       <c r="Q175" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R175" t="s">
         <v>19</v>
@@ -10271,7 +10268,7 @@
         <v>6.14447797958597</v>
       </c>
       <c r="Q176" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R176" t="s">
         <v>19</v>
@@ -10383,7 +10380,7 @@
         <v>6.92711887364308</v>
       </c>
       <c r="Q178" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R178" t="s">
         <v>19</v>
@@ -10439,7 +10436,7 @@
         <v>6.2354273391839</v>
       </c>
       <c r="Q179" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R179" t="s">
         <v>21</v>
@@ -10551,7 +10548,7 @@
         <v>6.63912975414038</v>
       </c>
       <c r="Q181" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R181" t="s">
         <v>22</v>
@@ -10719,7 +10716,7 @@
         <v>5.82468005360185</v>
       </c>
       <c r="Q184" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R184" t="s">
         <v>22</v>
@@ -10775,7 +10772,7 @@
         <v>6.2998174905953</v>
       </c>
       <c r="Q185" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R185" t="s">
         <v>19</v>
@@ -10831,7 +10828,7 @@
         <v>4.12665768434459</v>
       </c>
       <c r="Q186" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R186" t="s">
         <v>19</v>
@@ -10887,7 +10884,7 @@
         <v>5.67885249812224</v>
       </c>
       <c r="Q187" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R187" t="s">
         <v>21</v>
@@ -10999,7 +10996,7 @@
         <v>6.37064583412474</v>
       </c>
       <c r="Q189" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R189" t="s">
         <v>19</v>
@@ -11058,7 +11055,7 @@
         <v>18</v>
       </c>
       <c r="R190" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="191">
@@ -11167,7 +11164,7 @@
         <v>6.35701629810708</v>
       </c>
       <c r="Q192" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R192" t="s">
         <v>22</v>
@@ -11223,7 +11220,7 @@
         <v>5.60052154813252</v>
       </c>
       <c r="Q193" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R193" t="s">
         <v>22</v>
@@ -11335,7 +11332,7 @@
         <v>6.31673044735265</v>
       </c>
       <c r="Q195" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R195" t="s">
         <v>19</v>
@@ -11447,7 +11444,7 @@
         <v>6.17447164823771</v>
       </c>
       <c r="Q197" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R197" t="s">
         <v>19</v>
@@ -11503,7 +11500,7 @@
         <v>6.79499638379391</v>
       </c>
       <c r="Q198" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R198" t="s">
         <v>19</v>
@@ -11559,7 +11556,7 @@
         <v>6.41783323979847</v>
       </c>
       <c r="Q199" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R199" t="s">
         <v>22</v>
@@ -11671,7 +11668,7 @@
         <v>6.52686932283281</v>
       </c>
       <c r="Q201" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R201" t="s">
         <v>22</v>
@@ -11839,7 +11836,7 @@
         <v>7.24133634376239</v>
       </c>
       <c r="Q204" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R204" t="s">
         <v>19</v>
@@ -11895,7 +11892,7 @@
         <v>6.37269133992546</v>
       </c>
       <c r="Q205" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R205" t="s">
         <v>19</v>
@@ -12063,7 +12060,7 @@
         <v>6.53273211308114</v>
       </c>
       <c r="Q208" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R208" t="s">
         <v>22</v>
@@ -12175,7 +12172,7 @@
         <v>6.1252635960656</v>
       </c>
       <c r="Q210" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R210" t="s">
         <v>19</v>
@@ -12231,7 +12228,7 @@
         <v>6.10714035767981</v>
       </c>
       <c r="Q211" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R211" t="s">
         <v>19</v>
@@ -12287,7 +12284,7 @@
         <v>6.29418734831576</v>
       </c>
       <c r="Q212" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R212" t="s">
         <v>19</v>
@@ -12343,7 +12340,7 @@
         <v>6.0838457696563</v>
       </c>
       <c r="Q213" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R213" t="s">
         <v>22</v>
@@ -12399,7 +12396,7 @@
         <v>6.56030361141605</v>
       </c>
       <c r="Q214" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R214" t="s">
         <v>19</v>
@@ -12511,7 +12508,7 @@
         <v>6.33028041296208</v>
       </c>
       <c r="Q216" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R216" t="s">
         <v>19</v>
@@ -12567,7 +12564,7 @@
         <v>6.38373751785686</v>
       </c>
       <c r="Q217" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R217" t="s">
         <v>19</v>
@@ -12682,7 +12679,7 @@
         <v>20</v>
       </c>
       <c r="R219" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="220">
@@ -12735,7 +12732,7 @@
         <v>6.5507552160551</v>
       </c>
       <c r="Q220" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R220" t="s">
         <v>22</v>
@@ -12791,7 +12788,7 @@
         <v>5.86771085742456</v>
       </c>
       <c r="Q221" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R221" t="s">
         <v>19</v>
@@ -12903,7 +12900,7 @@
         <v>4.59526004677123</v>
       </c>
       <c r="Q223" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R223" t="s">
         <v>19</v>
@@ -13015,7 +13012,7 @@
         <v>6.77877394165246</v>
       </c>
       <c r="Q225" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R225" t="s">
         <v>22</v>
@@ -13127,7 +13124,7 @@
         <v>6.91139107545657</v>
       </c>
       <c r="Q227" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R227" t="s">
         <v>22</v>
@@ -13519,7 +13516,7 @@
         <v>6.64886240914619</v>
       </c>
       <c r="Q234" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R234" t="s">
         <v>19</v>
@@ -13575,7 +13572,7 @@
         <v>6.25120499237047</v>
       </c>
       <c r="Q235" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R235" t="s">
         <v>19</v>
@@ -13799,7 +13796,7 @@
         <v>6.32550473870376</v>
       </c>
       <c r="Q239" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R239" t="s">
         <v>19</v>
@@ -13911,7 +13908,7 @@
         <v>6.8303070640081</v>
       </c>
       <c r="Q241" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R241" t="s">
         <v>19</v>
@@ -14023,7 +14020,7 @@
         <v>6.52329758770792</v>
       </c>
       <c r="Q243" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R243" t="s">
         <v>19</v>
@@ -14191,7 +14188,7 @@
         <v>6.52500390325962</v>
       </c>
       <c r="Q246" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R246" t="s">
         <v>19</v>
@@ -14247,7 +14244,7 @@
         <v>5.6018183104173</v>
       </c>
       <c r="Q247" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R247" t="s">
         <v>19</v>
@@ -14583,7 +14580,7 @@
         <v>6.55370144222447</v>
       </c>
       <c r="Q253" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R253" t="s">
         <v>22</v>
@@ -14639,7 +14636,7 @@
         <v>6.65304391970138</v>
       </c>
       <c r="Q254" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R254" t="s">
         <v>21</v>
@@ -15143,7 +15140,7 @@
         <v>6.4435569859562</v>
       </c>
       <c r="Q263" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R263" t="s">
         <v>19</v>
@@ -15199,7 +15196,7 @@
         <v>6.43414619500887</v>
       </c>
       <c r="Q264" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R264" t="s">
         <v>22</v>
@@ -15255,7 +15252,7 @@
         <v>6.42688432488472</v>
       </c>
       <c r="Q265" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R265" t="s">
         <v>22</v>
@@ -15311,7 +15308,7 @@
         <v>7.04130313472114</v>
       </c>
       <c r="Q266" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R266" t="s">
         <v>22</v>
@@ -15367,7 +15364,7 @@
         <v>5.99922070346052</v>
       </c>
       <c r="Q267" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R267" t="s">
         <v>22</v>
@@ -15703,7 +15700,7 @@
         <v>6.3613207292199</v>
       </c>
       <c r="Q273" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R273" t="s">
         <v>22</v>
@@ -15759,7 +15756,7 @@
         <v>6.17034495493439</v>
       </c>
       <c r="Q274" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R274" t="s">
         <v>22</v>
@@ -15871,10 +15868,10 @@
         <v>6.46554908280383</v>
       </c>
       <c r="Q276" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R276" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="277">
@@ -15983,7 +15980,7 @@
         <v>6.58492554954646</v>
       </c>
       <c r="Q278" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R278" t="s">
         <v>19</v>
@@ -16039,7 +16036,7 @@
         <v>6.44591915713554</v>
       </c>
       <c r="Q279" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R279" t="s">
         <v>21</v>
@@ -16207,7 +16204,7 @@
         <v>6.19970195847384</v>
       </c>
       <c r="Q282" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R282" t="s">
         <v>22</v>
@@ -16263,7 +16260,7 @@
         <v>5.92953308251</v>
       </c>
       <c r="Q283" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R283" t="s">
         <v>22</v>
@@ -16319,7 +16316,7 @@
         <v>6.89479293046363</v>
       </c>
       <c r="Q284" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R284" t="s">
         <v>19</v>
@@ -16375,7 +16372,7 @@
         <v>6.7744413493394</v>
       </c>
       <c r="Q285" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R285" t="s">
         <v>19</v>
@@ -16431,7 +16428,7 @@
         <v>6.16388580224729</v>
       </c>
       <c r="Q286" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R286" t="s">
         <v>19</v>
@@ -16487,7 +16484,7 @@
         <v>6.51931708694556</v>
       </c>
       <c r="Q287" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R287" t="s">
         <v>22</v>
@@ -16543,7 +16540,7 @@
         <v>3.67736651862731</v>
       </c>
       <c r="Q288" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R288" t="s">
         <v>22</v>
@@ -16711,7 +16708,7 @@
         <v>6.40568112052239</v>
       </c>
       <c r="Q291" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R291" t="s">
         <v>22</v>
@@ -16767,7 +16764,7 @@
         <v>6.80141137362178</v>
       </c>
       <c r="Q292" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R292" t="s">
         <v>22</v>
@@ -17103,7 +17100,7 @@
         <v>5.81519589159046</v>
       </c>
       <c r="Q298" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R298" t="s">
         <v>21</v>
@@ -17159,7 +17156,7 @@
         <v>6.22783889059435</v>
       </c>
       <c r="Q299" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R299" t="s">
         <v>22</v>
@@ -17327,7 +17324,7 @@
         <v>5.92715951311017</v>
       </c>
       <c r="Q302" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R302" t="s">
         <v>21</v>
@@ -17495,7 +17492,7 @@
         <v>6.1485217182086</v>
       </c>
       <c r="Q305" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R305" t="s">
         <v>21</v>
@@ -17607,7 +17604,7 @@
         <v>6.63643375955574</v>
       </c>
       <c r="Q307" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R307" t="s">
         <v>21</v>
@@ -17719,7 +17716,7 @@
         <v>5.70998763410521</v>
       </c>
       <c r="Q309" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R309" t="s">
         <v>22</v>
@@ -17831,7 +17828,7 @@
         <v>6.69170659335512</v>
       </c>
       <c r="Q311" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R311" t="s">
         <v>22</v>
@@ -17887,7 +17884,7 @@
         <v>6.07704891920193</v>
       </c>
       <c r="Q312" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R312" t="s">
         <v>22</v>
@@ -17999,7 +17996,7 @@
         <v>6.13891462467098</v>
       </c>
       <c r="Q314" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R314" t="s">
         <v>19</v>
@@ -18055,7 +18052,7 @@
         <v>6.30026589972477</v>
       </c>
       <c r="Q315" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R315" t="s">
         <v>22</v>
@@ -18447,7 +18444,7 @@
         <v>6.54285353524833</v>
       </c>
       <c r="Q322" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R322" t="s">
         <v>22</v>
@@ -18503,7 +18500,7 @@
         <v>6.839168925427</v>
       </c>
       <c r="Q323" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R323" t="s">
         <v>19</v>
@@ -18727,7 +18724,7 @@
         <v>5.64857570805441</v>
       </c>
       <c r="Q327" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R327" t="s">
         <v>22</v>
@@ -18783,7 +18780,7 @@
         <v>6.27400546054578</v>
       </c>
       <c r="Q328" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R328" t="s">
         <v>19</v>
@@ -18842,7 +18839,7 @@
         <v>18</v>
       </c>
       <c r="R329" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="330">
@@ -18951,7 +18948,7 @@
         <v>6.40218559138605</v>
       </c>
       <c r="Q331" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R331" t="s">
         <v>19</v>
@@ -19063,7 +19060,7 @@
         <v>6.81928928305626</v>
       </c>
       <c r="Q333" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R333" t="s">
         <v>19</v>
@@ -19231,7 +19228,7 @@
         <v>6.53973310114962</v>
       </c>
       <c r="Q336" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R336" t="s">
         <v>19</v>
@@ -19567,7 +19564,7 @@
         <v>6.87328411321059</v>
       </c>
       <c r="Q342" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R342" t="s">
         <v>19</v>
@@ -19679,7 +19676,7 @@
         <v>6.61037837555831</v>
       </c>
       <c r="Q344" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R344" t="s">
         <v>19</v>
@@ -19850,7 +19847,7 @@
         <v>20</v>
       </c>
       <c r="R347" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="348">
@@ -20015,7 +20012,7 @@
         <v>6.74759772582764</v>
       </c>
       <c r="Q350" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R350" t="s">
         <v>19</v>
@@ -20242,7 +20239,7 @@
         <v>20</v>
       </c>
       <c r="R354" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="355">
@@ -20463,7 +20460,7 @@
         <v>5.68891838912333</v>
       </c>
       <c r="Q358" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R358" t="s">
         <v>22</v>
@@ -20631,7 +20628,7 @@
         <v>4.09383678482498</v>
       </c>
       <c r="Q361" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R361" t="s">
         <v>19</v>
@@ -20690,7 +20687,7 @@
         <v>18</v>
       </c>
       <c r="R362" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="363">
@@ -20799,7 +20796,7 @@
         <v>6.79284641929694</v>
       </c>
       <c r="Q364" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R364" t="s">
         <v>19</v>
@@ -20911,7 +20908,7 @@
         <v>6.11292038110893</v>
       </c>
       <c r="Q366" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R366" t="s">
         <v>19</v>
@@ -20967,7 +20964,7 @@
         <v>6.33102273015195</v>
       </c>
       <c r="Q367" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R367" t="s">
         <v>19</v>
@@ -21079,7 +21076,7 @@
         <v>5.88215899724782</v>
       </c>
       <c r="Q369" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R369" t="s">
         <v>19</v>
@@ -21194,7 +21191,7 @@
         <v>18</v>
       </c>
       <c r="R371" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="372">
@@ -21247,7 +21244,7 @@
         <v>6.51826754901867</v>
       </c>
       <c r="Q372" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R372" t="s">
         <v>19</v>
@@ -21471,7 +21468,7 @@
         <v>6.4530817040907</v>
       </c>
       <c r="Q376" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R376" t="s">
         <v>19</v>
@@ -21583,7 +21580,7 @@
         <v>6.44412582298139</v>
       </c>
       <c r="Q378" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R378" t="s">
         <v>21</v>
@@ -21639,7 +21636,7 @@
         <v>6.79899752947677</v>
       </c>
       <c r="Q379" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R379" t="s">
         <v>22</v>
@@ -21807,7 +21804,7 @@
         <v>6.13634245406924</v>
       </c>
       <c r="Q382" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R382" t="s">
         <v>19</v>
@@ -22311,7 +22308,7 @@
         <v>6.74500093354091</v>
       </c>
       <c r="Q391" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R391" t="s">
         <v>19</v>
@@ -22538,7 +22535,7 @@
         <v>20</v>
       </c>
       <c r="R395" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="396">
@@ -22759,7 +22756,7 @@
         <v>5.87656144125113</v>
       </c>
       <c r="Q399" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R399" t="s">
         <v>22</v>
@@ -22927,7 +22924,7 @@
         <v>4.19051103833038</v>
       </c>
       <c r="Q402" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R402" t="s">
         <v>19</v>
@@ -23095,7 +23092,7 @@
         <v>6.79470386940667</v>
       </c>
       <c r="Q405" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R405" t="s">
         <v>19</v>
@@ -23207,7 +23204,7 @@
         <v>6.17282414553498</v>
       </c>
       <c r="Q407" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R407" t="s">
         <v>19</v>
@@ -23263,7 +23260,7 @@
         <v>6.33243090484326</v>
       </c>
       <c r="Q408" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R408" t="s">
         <v>19</v>
@@ -23375,7 +23372,7 @@
         <v>5.87452456916606</v>
       </c>
       <c r="Q410" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R410" t="s">
         <v>22</v>
@@ -23543,10 +23540,10 @@
         <v>6.51880946775874</v>
       </c>
       <c r="Q413" t="s">
+        <v>23</v>
+      </c>
+      <c r="R413" t="s">
         <v>24</v>
-      </c>
-      <c r="R413" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="414">
@@ -23767,7 +23764,7 @@
         <v>6.45231623259536</v>
       </c>
       <c r="Q417" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R417" t="s">
         <v>19</v>
@@ -23879,7 +23876,7 @@
         <v>6.44199227643571</v>
       </c>
       <c r="Q419" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R419" t="s">
         <v>21</v>
@@ -23935,7 +23932,7 @@
         <v>6.80016476038165</v>
       </c>
       <c r="Q420" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R420" t="s">
         <v>22</v>
@@ -24103,7 +24100,7 @@
         <v>6.1333870620253</v>
       </c>
       <c r="Q423" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R423" t="s">
         <v>19</v>

</xml_diff>